<commit_message>
update dissertation award + CE committee
</commit_message>
<xml_diff>
--- a/about/Leadership_2024-25.xlsx
+++ b/about/Leadership_2024-25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emma/docs/apls-org/about/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54DBA143-B025-C245-A02B-4B6B1977B9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2A7D49-B6E6-104A-866F-8D7E673E0439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28000" yWindow="-1000" windowWidth="25600" windowHeight="26580" firstSheet="13" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="17640" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Book" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="447">
   <si>
     <t>Position</t>
   </si>
@@ -871,12 +871,6 @@
     <t>bennett.mts@gmail.com</t>
   </si>
   <si>
-    <t>Erik Davis</t>
-  </si>
-  <si>
-    <t>kiresivad1@aol.com</t>
-  </si>
-  <si>
     <t>Joni E. Johnston</t>
   </si>
   <si>
@@ -1388,6 +1382,9 @@
   </si>
   <si>
     <t>Member (Awards Sub Committee)</t>
+  </si>
+  <si>
+    <t>Tate Madison</t>
   </si>
 </sst>
 </file>
@@ -1815,7 +1812,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>123</v>
@@ -1843,10 +1840,10 @@
         <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D4" t="s">
         <v>243</v>
@@ -1857,10 +1854,10 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D5" t="s">
         <v>38</v>
@@ -1910,7 +1907,7 @@
         <v>104</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>125</v>
@@ -1955,7 +1952,7 @@
         <v>132</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>38</v>
@@ -1980,10 +1977,10 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C7" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D7" t="s">
         <v>243</v>
@@ -2044,7 +2041,7 @@
         <v>137</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>32</v>
@@ -2072,7 +2069,7 @@
         <v>140</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>32</v>
@@ -2125,10 +2122,10 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C9" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D9" t="s">
         <v>243</v>
@@ -2139,7 +2136,7 @@
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C10" t="s">
         <v>244</v>
@@ -2153,10 +2150,10 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C11" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D11" t="s">
         <v>243</v>
@@ -2228,10 +2225,10 @@
         <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>243</v>
@@ -2245,7 +2242,7 @@
         <v>147</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -2270,10 +2267,10 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C7" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D7" t="s">
         <v>243</v>
@@ -2326,7 +2323,7 @@
         <v>259</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2337,7 +2334,7 @@
         <v>151</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>32</v>
@@ -2349,10 +2346,10 @@
         <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>36</v>
@@ -2360,13 +2357,13 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>152</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>36</v>
@@ -2377,10 +2374,10 @@
         <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>36</v>
@@ -2388,13 +2385,13 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>153</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>36</v>
@@ -2402,13 +2399,13 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>243</v>
@@ -2419,10 +2416,10 @@
         <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>243</v>
@@ -2433,10 +2430,10 @@
         <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>243</v>
@@ -2461,10 +2458,10 @@
         <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>243</v>
@@ -2475,10 +2472,10 @@
         <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>243</v>
@@ -2536,13 +2533,13 @@
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>361</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2603,13 +2600,13 @@
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>161</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>36</v>
@@ -2631,13 +2628,13 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>165</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>38</v>
@@ -2651,7 +2648,7 @@
         <v>158</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>32</v>
@@ -2673,13 +2670,13 @@
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B13" t="s">
         <v>170</v>
       </c>
       <c r="C13" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D13" t="s">
         <v>38</v>
@@ -2723,10 +2720,10 @@
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -2738,7 +2735,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2762,7 +2759,7 @@
         <v>172</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2821,7 +2818,7 @@
         <v>175</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>38</v>
@@ -2852,7 +2849,7 @@
         <v>179</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2919,7 +2916,7 @@
         <v>188</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>38</v>
@@ -2936,7 +2933,7 @@
         <v>190</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2944,10 +2941,10 @@
         <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>243</v>
@@ -2979,7 +2976,7 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
@@ -3019,13 +3016,13 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>38</v>
@@ -3034,13 +3031,13 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>220</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>38</v>
@@ -3049,13 +3046,13 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>38</v>
@@ -3064,13 +3061,13 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>38</v>
@@ -3079,13 +3076,13 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>38</v>
@@ -3094,13 +3091,13 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>38</v>
@@ -3109,13 +3106,13 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>38</v>
@@ -3124,13 +3121,13 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B10" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C10" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D10" t="s">
         <v>38</v>
@@ -3139,13 +3136,13 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B11" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C11" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D11" t="s">
         <v>38</v>
@@ -3154,13 +3151,13 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B12" t="s">
         <v>83</v>
       </c>
       <c r="C12" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D12" t="s">
         <v>38</v>
@@ -3169,13 +3166,13 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B13" t="s">
         <v>175</v>
       </c>
       <c r="C13" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D13" t="s">
         <v>38</v>
@@ -3184,10 +3181,10 @@
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B14" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C14" t="s">
         <v>130</v>
@@ -3251,7 +3248,7 @@
         <v>223</v>
       </c>
       <c r="C3" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>243</v>
@@ -3262,10 +3259,10 @@
         <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C4" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>38</v>
@@ -3276,10 +3273,10 @@
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C5" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>243</v>
@@ -3687,7 +3684,7 @@
         <v>172</v>
       </c>
       <c r="C2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>38</v>
@@ -3698,10 +3695,10 @@
         <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C3" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>249</v>
@@ -3751,7 +3748,7 @@
         <v>226</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>249</v>
@@ -3776,10 +3773,10 @@
         <v>227</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>249</v>
@@ -3790,10 +3787,10 @@
         <v>228</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>249</v>
@@ -3818,10 +3815,10 @@
         <v>233</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>249</v>
@@ -3832,10 +3829,10 @@
         <v>234</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>249</v>
@@ -3846,10 +3843,10 @@
         <v>235</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>249</v>
@@ -3860,10 +3857,10 @@
         <v>236</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>249</v>
@@ -3927,7 +3924,7 @@
         <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>38</v>
@@ -3935,13 +3932,13 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>198</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>38</v>
@@ -3955,7 +3952,7 @@
         <v>69</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>243</v>
@@ -3969,7 +3966,7 @@
         <v>195</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>36</v>
@@ -3997,7 +3994,7 @@
         <v>238</v>
       </c>
       <c r="C7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>38</v>
@@ -4008,10 +4005,10 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D8" t="s">
         <v>38</v>
@@ -4022,10 +4019,10 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C9" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D9" t="s">
         <v>243</v>
@@ -4036,10 +4033,10 @@
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C10" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D10" t="s">
         <v>243</v>
@@ -4050,10 +4047,10 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C11" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D11" t="s">
         <v>243</v>
@@ -4064,10 +4061,10 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C12" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D12" t="s">
         <v>243</v>
@@ -4078,10 +4075,10 @@
         <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D13" t="s">
         <v>243</v>
@@ -4095,7 +4092,7 @@
         <v>149</v>
       </c>
       <c r="C14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D14" t="s">
         <v>243</v>
@@ -4103,13 +4100,13 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B15" t="s">
+        <v>399</v>
+      </c>
+      <c r="C15" t="s">
         <v>400</v>
-      </c>
-      <c r="B15" t="s">
-        <v>401</v>
-      </c>
-      <c r="C15" t="s">
-        <v>402</v>
       </c>
       <c r="D15" t="s">
         <v>249</v>
@@ -4117,13 +4114,13 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B16" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C16" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D16" t="s">
         <v>249</v>
@@ -4131,13 +4128,13 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B17" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C17" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D17" t="s">
         <v>249</v>
@@ -4298,7 +4295,7 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>166</v>
@@ -4393,7 +4390,7 @@
         <v>220</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>38</v>
@@ -4407,7 +4404,7 @@
         <v>196</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>36</v>
@@ -4421,7 +4418,7 @@
         <v>223</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>36</v>
@@ -4435,7 +4432,7 @@
         <v>199</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>38</v>
@@ -4560,9 +4557,9 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4704,7 +4701,7 @@
         <v>276</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>243</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4712,13 +4709,10 @@
         <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>278</v>
+        <v>446</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>243</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -4756,7 +4750,7 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>78</v>
@@ -4770,7 +4764,7 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>83</v>
@@ -4801,7 +4795,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>82</v>
@@ -4857,13 +4851,13 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
+        <v>279</v>
+      </c>
+      <c r="C9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D9" t="s">
         <v>281</v>
-      </c>
-      <c r="C9" t="s">
-        <v>282</v>
-      </c>
-      <c r="D9" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4874,10 +4868,10 @@
         <v>194</v>
       </c>
       <c r="C10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4885,10 +4879,10 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D11" t="s">
         <v>36</v>
@@ -4899,13 +4893,13 @@
         <v>110</v>
       </c>
       <c r="B12" t="s">
+        <v>285</v>
+      </c>
+      <c r="C12" t="s">
+        <v>286</v>
+      </c>
+      <c r="D12" t="s">
         <v>287</v>
-      </c>
-      <c r="C12" t="s">
-        <v>288</v>
-      </c>
-      <c r="D12" t="s">
-        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -4949,7 +4943,7 @@
         <v>63</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>38</v>
@@ -4971,13 +4965,13 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>36</v>
@@ -5005,7 +4999,7 @@
         <v>93</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>38</v>
@@ -5019,7 +5013,7 @@
         <v>94</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>38</v>
@@ -5086,10 +5080,10 @@
         <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>38</v>
@@ -5100,10 +5094,10 @@
         <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>243</v>
@@ -5114,10 +5108,10 @@
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>243</v>
@@ -5128,10 +5122,10 @@
         <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>243</v>
@@ -5142,10 +5136,10 @@
         <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>243</v>
@@ -5200,13 +5194,13 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>38</v>
@@ -5220,7 +5214,7 @@
         <v>239</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>36</v>
@@ -5234,7 +5228,7 @@
         <v>103</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>36</v>
@@ -5270,7 +5264,7 @@
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>108</v>
@@ -5290,7 +5284,7 @@
         <v>240</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>243</v>
@@ -5304,7 +5298,7 @@
         <v>241</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>243</v>
@@ -5318,7 +5312,7 @@
         <v>242</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>243</v>
@@ -5390,10 +5384,10 @@
         <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>243</v>
@@ -5479,10 +5473,10 @@
         <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>38</v>
@@ -5507,7 +5501,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -5524,7 +5518,7 @@
         <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>243</v>
@@ -5538,7 +5532,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D7" t="s">
         <v>243</v>
@@ -5549,7 +5543,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>

</xml_diff>